<commit_message>
Updated presentation and excel file
</commit_message>
<xml_diff>
--- a/MESSAGEix_South_Africa/Data/SSP5/Summary_for_plots.xlsx
+++ b/MESSAGEix_South_Africa/Data/SSP5/Summary_for_plots.xlsx
@@ -8,93 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Documents/GitHub/SSP5/MESSAGEix_South_Africa/Data/SSP5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05632109-168F-C743-9100-93EE18048B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ECB349-0798-7B47-BF9D-52CBB55C8FC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{8898456C-A78B-7F41-96FB-4F0903FF66C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$A$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$A$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$A$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$A$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$A$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$A$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$A$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$A$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$A$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$A$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$A$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$A$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$A$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$A$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$A$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$A$7</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$A$8</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$B$1:$G$3</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$B$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$B$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$B$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$B$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$B$8:$G$8</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Sheet1!$F$2:$F$8</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Sheet1!$G$2:$G$8</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v2.38" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v2.39" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v2.40" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v2.41" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v2.42" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v2.43" hidden="1">Sheet1!$A$7</definedName>
-    <definedName name="_xlchart.v2.44" hidden="1">Sheet1!$A$8</definedName>
-    <definedName name="_xlchart.v2.45" hidden="1">Sheet1!$B$1:$G$1</definedName>
-    <definedName name="_xlchart.v2.46" hidden="1">Sheet1!$B$2:$G$2</definedName>
-    <definedName name="_xlchart.v2.47" hidden="1">Sheet1!$B$3:$G$3</definedName>
-    <definedName name="_xlchart.v2.48" hidden="1">Sheet1!$B$4:$G$4</definedName>
-    <definedName name="_xlchart.v2.49" hidden="1">Sheet1!$B$5:$G$5</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v2.50" hidden="1">Sheet1!$B$6:$G$6</definedName>
-    <definedName name="_xlchart.v2.51" hidden="1">Sheet1!$B$7:$G$7</definedName>
-    <definedName name="_xlchart.v2.52" hidden="1">Sheet1!$B$8:$G$8</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Sheet1!$E$2:$E$8</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -232,6 +152,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Useful Energy Demand [GWa]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -291,8 +236,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -384,8 +344,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -477,8 +452,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -570,8 +560,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -663,8 +668,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -756,8 +776,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -826,13 +861,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="704648415"/>
         <c:axId val="704650047"/>
@@ -953,7 +990,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1580,16 +1617,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1916,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F09893-A660-7F48-ADA1-440A4DA9A336}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>